<commit_message>
changes in UAT LIST 2 done
</commit_message>
<xml_diff>
--- a/mainadminhtml/samplefile/MIS/upsitypeclassify.xlsx
+++ b/mainadminhtml/samplefile/MIS/upsitypeclassify.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\future\mainadminhtml\samplefile\MIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\drreddys\mainadminhtml\samplefile\MIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name Of Upsi</t>
   </si>
@@ -39,19 +39,65 @@
   </si>
   <si>
     <t>Added By</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>Any other legal identifier</t>
+  </si>
+  <si>
+    <t>Any other legal identification number</t>
+  </si>
+  <si>
+    <t>Aadhaar</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Educational Qualification</t>
+  </si>
+  <si>
+    <t>Institute From Which Acquired</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Holdings In Shares</t>
+  </si>
+  <si>
+    <t>Holdings In ADRs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,9 +415,20 @@
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="37.5703125" customWidth="1"/>
+    <col min="14" max="14" width="42.42578125" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -385,9 +443,49 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>